<commit_message>
failed_stories && UP confidence by adding exemples to NLU
</commit_message>
<xml_diff>
--- a/bot/languages/en/results/confusion_table.xlsx
+++ b/bot/languages/en/results/confusion_table.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,18 +463,18 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>prevention_measures</t>
+          <t>vocative_thank_you</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>prevention_general</t>
+          <t>comment_positive</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -484,57 +484,57 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>vocative_thank_you</t>
+          <t>features_date</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>comment_positive</t>
+          <t>user_love</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>coronavirus_info</t>
+          <t>covid_worry</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>covid_info</t>
+          <t>user_scared</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>user_no_further_questions</t>
+          <t>covid_origins</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>vocative_thank_you</t>
+          <t>covid_info</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>user_love</t>
+          <t>bot_capabilities</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>features_date</t>
+          <t>vocative_call</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -544,12 +544,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>comment_positive</t>
+          <t>covid_dangerous</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>user_love</t>
+          <t>spread_risk</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -559,27 +559,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>test_virus</t>
+          <t>bot_personal_questions</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>test_who</t>
+          <t>bot_residence</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>spread_risk</t>
+          <t>bot_capabilities</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>covid_dangerous</t>
+          <t>vocative_help</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -589,12 +589,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bot_sing</t>
+          <t>prevention_home</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>bot_music</t>
+          <t>prevention_medical_attention</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -604,12 +604,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>bot_sexual</t>
+          <t>bot_residence</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>bot_personal_questions</t>
+          <t>bot_origin</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -619,12 +619,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>vocative_call</t>
+          <t>comment_positive</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>cc_lets_talk</t>
+          <t>comment_smart</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -634,12 +634,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>vocative_call</t>
+          <t>bot_sexual</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>comment_negative</t>
+          <t>bot_personal_questions</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -649,12 +649,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>bot_residence</t>
+          <t>vocative_call</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>bot_origin</t>
+          <t>cc_lets_talk</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -664,12 +664,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>bot_residence</t>
+          <t>covid_info</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>bot_personal_questions</t>
+          <t>covid_origins</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -679,12 +679,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>bot_capabilities</t>
+          <t>vocative_call</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>vocative_help</t>
+          <t>user_friend</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -694,12 +694,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>covid_food</t>
+          <t>covid_duration</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>spread_surfaces_food_objects</t>
+          <t>covid_crisis_howlong</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -709,12 +709,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>prevention_medical_attention</t>
+          <t>covid_duration</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>prevention_home</t>
+          <t>covid_info</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -724,12 +724,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>vocative_help</t>
+          <t>vocative_yes</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>vocative_call</t>
+          <t>country</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -739,12 +739,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>covid_duration</t>
+          <t>vocative_no</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>covid_info</t>
+          <t>comment_negative</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -754,12 +754,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>covid_duration</t>
+          <t>greeting_hello</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>covid_crisis_howlong</t>
+          <t>start</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -769,12 +769,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>spread_pets</t>
+          <t>quaratine_how_it_works</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>covid_surfaces</t>
+          <t>quarantine_general</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -789,7 +789,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>prevention_medical_attention</t>
+          <t>comment_negative</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -799,12 +799,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>bot_personality</t>
+          <t>covid_situation_last_update</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>bot_capabilities</t>
+          <t>country</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -814,12 +814,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>covid_symptoms</t>
+          <t>bot_name</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>prevention_medical_attention</t>
+          <t>bot_capabilities</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -829,12 +829,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>comment_offense</t>
+          <t>bot_name</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>comment_negative</t>
+          <t>bot_personal_questions</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -844,12 +844,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>covid_treatment</t>
+          <t>covid_crisis_howlong</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>prevention_medicine</t>
+          <t>spread_general</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -859,12 +859,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>prevention_measures</t>
+          <t>covid_symptoms</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>prevention_medical_attention</t>
+          <t>test_virus</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -874,12 +874,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>covid_situation</t>
+          <t>bot_personality</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>covid_current_statistics</t>
+          <t>bot_capabilities</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -889,12 +889,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>bot_sexual</t>
+          <t>spread_risk</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>bot_music</t>
+          <t>spread_general</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -904,12 +904,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>user_happy</t>
+          <t>comment_racist</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>cc_philosophical</t>
+          <t>comment_offense</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -919,12 +919,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>bot_music</t>
+          <t>comment_racist</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>comment_positive</t>
+          <t>cc_geography</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -934,12 +934,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>bot_music</t>
+          <t>bot_sing</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>bot_sing</t>
+          <t>bot_personal_questions</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -949,12 +949,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>covid_crisis_howlong</t>
+          <t>covid_treatment</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>spread_general</t>
+          <t>prevention_medicine</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -964,12 +964,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>bot_personal_questions</t>
+          <t>covid_info</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>bot_residence</t>
+          <t>coronavirus_info</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -979,12 +979,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>prevention_medicine</t>
+          <t>covid_origins</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>covid_treatment</t>
+          <t>cc_philosophical</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -994,12 +994,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>bot_appearance</t>
+          <t>user_particles</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>bot_personal_questions</t>
+          <t>comment_smart</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1009,12 +1009,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>vocative_sorry</t>
+          <t>user_particles</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>comment_negative</t>
+          <t>vocative_you_welcome</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1024,12 +1024,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>cc_newspaper</t>
+          <t>comment_negative</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>covid_origins</t>
+          <t>comment_offense</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1039,12 +1039,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>cc_philosophical</t>
+          <t>comment_negative</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>spread_animals</t>
+          <t>bot_capabilities</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1054,12 +1054,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>cc_philosophical</t>
+          <t>bot_personal_questions</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>cc_religion</t>
+          <t>user_love</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1069,12 +1069,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>quarantine_general</t>
+          <t>prevention_medical_attention</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>quaratine_how_it_works</t>
+          <t>covid_procedure_after_infection</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1084,12 +1084,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>comment_negative</t>
+          <t>prevention_medical_attention</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>bot_capabilities</t>
+          <t>covid_symptoms</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1099,12 +1099,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>comment_negative</t>
+          <t>cc_philosophical</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>vocative_call</t>
+          <t>features_time</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1114,12 +1114,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>covid_incubation</t>
+          <t>cc_philosophical</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>covid_symptoms</t>
+          <t>user_love</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1129,12 +1129,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>covid_procedure_after_infection</t>
+          <t>bot_music</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>prevention_medical_attention</t>
+          <t>bot_sing</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1144,12 +1144,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>covid_preexisting_illness</t>
+          <t>test_who</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>covid_mortality_rate</t>
+          <t>test_virus</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1159,165 +1159,15 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>covid_worry</t>
+          <t>covid_symptoms</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>user_scared</t>
+          <t>prevention_medical_attention</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>cc_lets_talk</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>bot_capabilities</t>
-        </is>
-      </c>
-      <c r="C50" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>covid_schools</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>prevention_general</t>
-        </is>
-      </c>
-      <c r="C51" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>bot_sing</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>bot_personal_questions</t>
-        </is>
-      </c>
-      <c r="C52" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>covid_info</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>covid_origins</t>
-        </is>
-      </c>
-      <c r="C53" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>spread_general</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>covid_origins</t>
-        </is>
-      </c>
-      <c r="C54" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>user_no_further_questions</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>vocative_help</t>
-        </is>
-      </c>
-      <c r="C55" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>bot_personal_questions</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>bot_sexual</t>
-        </is>
-      </c>
-      <c r="C56" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>user_particles</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>comment_smart</t>
-        </is>
-      </c>
-      <c r="C57" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>covid_worry</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>covid_mortality_rate</t>
-        </is>
-      </c>
-      <c r="C58" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>greeting_hello</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>start</t>
-        </is>
-      </c>
-      <c r="C59" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add 'the' to some covid_situation
</commit_message>
<xml_diff>
--- a/bot/languages/en/results/confusion_table.xlsx
+++ b/bot/languages/en/results/confusion_table.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,177 +454,177 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>vocative_thank_you</t>
+          <t>prevention_vaccine</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>comment_positive</t>
+          <t>prevention_medicine</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>13</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>comment_positive</t>
+          <t>prevention_medicine</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>vocative_thank_you</t>
+          <t>prevention_vaccine</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>vocative_call</t>
+          <t>vocative_thank_you</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>cc_lets_talk</t>
+          <t>comment_positive</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>test_virus</t>
+          <t>comment_positive</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>test_who</t>
+          <t>vocative_thank_you</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>prevention_home</t>
+          <t>test_who</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>prevention_medical_attention</t>
+          <t>test_virus</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>spread_surfaces_food_objects</t>
+          <t>vocative_help</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>covid_food</t>
+          <t>bot_capabilities</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>covid_origins</t>
+          <t>comment_offense</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>covid_info</t>
+          <t>comment_negative</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>bot_capabilities</t>
+          <t>prevention_home</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>vocative_call</t>
+          <t>prevention_medical_attention</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>covid_info</t>
+          <t>user_no_further_questions</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>coronavirus_info</t>
+          <t>vocative_thank_you</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>features_date</t>
+          <t>covid_origins</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>user_love</t>
+          <t>covid_duration</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>bot_sexual</t>
+          <t>cc_philosophical</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>bot_personal_questions</t>
+          <t>cc_religion</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>bot_personal_questions</t>
+          <t>bot_residence</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>bot_residence</t>
+          <t>bot_origin</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -634,12 +634,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>vocative_help</t>
+          <t>comment_negative</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>vocative_call</t>
+          <t>vocative_sorry</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -649,12 +649,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>comment_positive</t>
+          <t>covid_info</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>comment_smart</t>
+          <t>covid_duration</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -664,12 +664,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>user_scared</t>
+          <t>covid_current_statistics</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>covid_worry</t>
+          <t>covid_info</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -679,162 +679,162 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>comment_smart</t>
+          <t>quarantine_general</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>greeting_how_are_you</t>
+          <t>quaratine_how_it_works</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>comment_offense</t>
+          <t>covid_treatment</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>comment_negative</t>
+          <t>prevention_medicine</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>bot_residence</t>
+          <t>bot_sexual</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>bot_origin</t>
+          <t>bot_personal_questions</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>quaratine_how_it_works</t>
+          <t>vocative_call</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>quarantine_general</t>
+          <t>cc_lets_talk</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>cc_philosophical</t>
+          <t>cc_religion</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>features_time</t>
+          <t>bot_personal_questions</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>user_happy</t>
+          <t>prevention_medical_attention</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>cc_philosophical</t>
+          <t>covid_symptoms</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>user_happy</t>
+          <t>bot_residence</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>bot_games</t>
+          <t>bot_personal_questions</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>bot_sing</t>
+          <t>cc_philosophical</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>bot_personal_questions</t>
+          <t>bot_goal</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>bot_origin</t>
+          <t>covid_info</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>bot_residence</t>
+          <t>covid_origins</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>prevention_medical_attention</t>
+          <t>comment_smart</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>bot_personal_questions</t>
+          <t>bot_personality</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>prevention_medical_attention</t>
+          <t>coronavirus_info</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>covid_procedure_after_infection</t>
+          <t>covid_situation_last_update</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -844,12 +844,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>bot_residence</t>
+          <t>mask_general</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>bot_personal_questions</t>
+          <t>mask_use_put</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -859,12 +859,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>covid_schools</t>
+          <t>covid_dangerous</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>prevention_general</t>
+          <t>spread_risk</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -874,12 +874,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>country</t>
+          <t>user_love</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>bot_games</t>
+          <t>cc_philosophical</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -889,12 +889,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>greeting_how_are_you</t>
+          <t>bot_sing</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>user_particles</t>
+          <t>bot_personal_questions</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -904,12 +904,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>start</t>
+          <t>user_particles</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>greeting_hello</t>
+          <t>comment_negative</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -919,12 +919,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>bot_capabilities</t>
+          <t>comment_offense</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>bot_personality</t>
+          <t>comment_racist</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -934,12 +934,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>comment_negative</t>
+          <t>bot_appearance</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>bot_origin</t>
+          <t>bot_sexual</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -949,12 +949,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>prevention_home</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
           <t>comment_negative</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>comment_offense</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -964,12 +964,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>bot_sexual</t>
+          <t>vocative_you_welcome</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>user_love</t>
+          <t>vocative_no</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -979,12 +979,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>bot_personality</t>
+          <t>covid_symptoms</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>comment_positive</t>
+          <t>prevention_medical_attention</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -994,12 +994,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>bot_personality</t>
+          <t>greeting_hello</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>comment_smart</t>
+          <t>start</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1009,12 +1009,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>covid_situation_infected</t>
+          <t>greeting_hello</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>covid_situation</t>
+          <t>greeting_goodbye</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1024,12 +1024,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>covid_info</t>
+          <t>bot_appearance</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>covid_duration</t>
+          <t>bot_personal_questions</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1039,12 +1039,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>vocative_call</t>
+          <t>bot_music</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>comment_negative</t>
+          <t>bot_sing</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1054,12 +1054,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>covid_duration</t>
+          <t>features_date</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>covid_info</t>
+          <t>user_love</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1069,12 +1069,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>covid_symptoms</t>
+          <t>bot_capabilities</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>prevention_medical_attention</t>
+          <t>bot_name</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1084,12 +1084,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>greeting_hello</t>
+          <t>prevention_general</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>greeting_goodbye</t>
+          <t>bot_capabilities</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1114,12 +1114,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>prevention_medicine</t>
+          <t>bot_personal_questions</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>covid_treatment</t>
+          <t>bot_residence</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1129,12 +1129,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>cc_philosophical</t>
+          <t>covid_situation_infected</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>bot_name</t>
+          <t>covid_situation</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1144,15 +1144,255 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
+          <t>cc_religion</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>comment_negative</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>covid_worry</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>user_friend</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>greeting_how_are_you</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>bot_personality</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>prevention_medical_attention</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>covid_procedure_after_infection</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>vocative_help</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>vocative_call</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>bot_capabilities</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>greeting_goodbye</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
           <t>covid_crisis_howlong</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>covid_duration</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>user_scared</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>covid_worry</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>bot_name</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>bot_personal_questions</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>bot_real</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>comment_negative</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>covid_meaning</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>covid_info</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>vocative_call</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>comment_negative</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>covid_origins</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
         <is>
           <t>spread_general</t>
         </is>
       </c>
-      <c r="C48" t="n">
+      <c r="C60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>covid_food</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>spread_surfaces_food_objects</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>prevention_medicine</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>covid_treatment</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>covid_crisis_howlong</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>spread_general</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>comment_positive</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>comment_smart</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>